<commit_message>
ng: updatd pretas form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Nigeria/ng_lf_pretas_2_participant_202102.xlsx
+++ b/LF/PreTAS/Nigeria/ng_lf_pretas_2_participant_202102.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Nigeria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448E76FA-DD80-486C-A1FE-3BAE425FFB86}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE2A684-6868-45BB-BE40-30B1B4B725ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -317,9 +317,6 @@
     <t>ng_lf_pretas_2_participant_202102</t>
   </si>
   <si>
-    <t>2. Nigeria - Pre TAS FL Participants Form</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>concat(${p_recorder_id}, '-', ${p_cluster_id}, '-', ${p_id_sequence})</t>
+  </si>
+  <si>
+    <t>2. Nigeria - Pre TAS LF Participants Form</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -899,7 +899,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>18</v>
@@ -936,14 +936,14 @@
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>98</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="8"/>
@@ -966,11 +966,11 @@
         <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="8"/>
@@ -993,11 +993,11 @@
         <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8"/>
@@ -1021,11 +1021,11 @@
         <v>84</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="8"/>
@@ -1220,7 +1220,7 @@
         <v>75</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>78</v>
@@ -1421,8 +1421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1449,7 +1449,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B2" t="s">
         <v>94</v>
@@ -1458,7 +1458,7 @@
         <v>20210216</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ng: update nigeria forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Nigeria/ng_lf_pretas_2_participant_202102.xlsx
+++ b/LF/PreTAS/Nigeria/ng_lf_pretas_2_participant_202102.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\LF\PreTAS\Nigeria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEE2A684-6868-45BB-BE40-30B1B4B725ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF16480C-6395-444E-8601-2DA98D39F5AE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -314,9 +314,6 @@
     <t>p_code_id</t>
   </si>
   <si>
-    <t>ng_lf_pretas_2_participant_202102</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -353,7 +350,10 @@
     <t>concat(${p_recorder_id}, '-', ${p_cluster_id}, '-', ${p_id_sequence})</t>
   </si>
   <si>
-    <t>2. Nigeria - Pre TAS LF Participants Form</t>
+    <t>2. Nigeria - Pre TAS LF Participants Form V2</t>
+  </si>
+  <si>
+    <t>ng_lf_pretas_2_participant_202102_v2</t>
   </si>
 </sst>
 </file>
@@ -814,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L13" sqref="L13"/>
@@ -899,7 +899,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>18</v>
@@ -936,14 +936,14 @@
         <v>28</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="8"/>
@@ -966,11 +966,11 @@
         <v>83</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="8"/>
@@ -993,11 +993,11 @@
         <v>39</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F5" s="4"/>
       <c r="G5" s="8"/>
@@ -1021,11 +1021,11 @@
         <v>84</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="8"/>
@@ -1220,7 +1220,7 @@
         <v>75</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>78</v>
@@ -1421,14 +1421,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.875" bestFit="1" customWidth="1"/>
   </cols>
@@ -1449,16 +1449,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" t="s">
         <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>94</v>
       </c>
       <c r="C2">
         <v>20210216</v>
       </c>
       <c r="D2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>